<commit_message>
6 YN and revised 3
Cool couple graphs with facet_grid
</commit_message>
<xml_diff>
--- a/Diccionario.xlsx
+++ b/Diccionario.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\elave\Documents\GitHub\R\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{91FEF750-792F-40D5-88DA-2D4794FC5E1E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76FD4E1D-9F54-4537-BBA4-0F9E3AFFB4EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{86D663B0-B964-4625-B9D2-5A0636F90473}"/>
   </bookViews>
@@ -593,7 +593,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -620,6 +620,13 @@
       <b/>
       <sz val="14"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="0" tint="-0.249977111117893"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -797,7 +804,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -824,75 +831,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -916,6 +854,78 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="8" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1233,8 +1243,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B4D3EEAC-ABE6-4FBE-8671-3572004B2C97}">
   <dimension ref="A1:G178"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="D160" sqref="D160"/>
+    <sheetView tabSelected="1" topLeftCell="A130" workbookViewId="0">
+      <selection activeCell="C162" sqref="C162"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -1263,7 +1273,7 @@
       <c r="E1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="G1" s="37">
+      <c r="G1" s="14">
         <v>3</v>
       </c>
     </row>
@@ -1279,16 +1289,16 @@
       </c>
       <c r="D2" s="3"/>
       <c r="E2" s="3"/>
-      <c r="G2" s="38"/>
+      <c r="G2" s="15"/>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A3" s="14" t="s">
+      <c r="A3" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="20" t="s">
+      <c r="C3" s="37" t="s">
         <v>2</v>
       </c>
       <c r="D3" s="4">
@@ -1297,32 +1307,32 @@
       <c r="E3" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="G3" s="39">
+      <c r="G3" s="16">
         <v>4</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="16"/>
-      <c r="B4" s="24"/>
-      <c r="C4" s="22"/>
+      <c r="A4" s="24"/>
+      <c r="B4" s="26"/>
+      <c r="C4" s="39"/>
       <c r="D4" s="5">
         <v>2</v>
       </c>
       <c r="E4" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="G4" s="40" t="s">
+      <c r="G4" s="17" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A5" s="14" t="s">
+      <c r="A5" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B5" s="14" t="s">
+      <c r="B5" s="22" t="s">
         <v>14</v>
       </c>
-      <c r="C5" s="20" t="s">
+      <c r="C5" s="37" t="s">
         <v>13</v>
       </c>
       <c r="D5" s="4">
@@ -1331,32 +1341,32 @@
       <c r="E5" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="G5" s="41">
+      <c r="G5" s="18">
         <v>5</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="15" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="16"/>
-      <c r="B6" s="16"/>
-      <c r="C6" s="22"/>
+      <c r="A6" s="24"/>
+      <c r="B6" s="24"/>
+      <c r="C6" s="39"/>
       <c r="D6" s="5">
         <v>2</v>
       </c>
       <c r="E6" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="G6" s="42" t="s">
+      <c r="G6" s="19" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A7" s="14" t="s">
+      <c r="A7" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="17" t="s">
+      <c r="B7" s="30" t="s">
         <v>31</v>
       </c>
-      <c r="C7" s="20" t="s">
+      <c r="C7" s="37" t="s">
         <v>17</v>
       </c>
       <c r="D7" s="4">
@@ -1365,28 +1375,28 @@
       <c r="E7" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="G7" s="43">
+      <c r="G7" s="20">
         <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="15"/>
-      <c r="B8" s="18"/>
-      <c r="C8" s="21"/>
+      <c r="A8" s="23"/>
+      <c r="B8" s="44"/>
+      <c r="C8" s="38"/>
       <c r="D8" s="6">
         <v>1</v>
       </c>
       <c r="E8" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="G8" s="44" t="s">
+      <c r="G8" s="21" t="s">
         <v>101</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="15"/>
-      <c r="B9" s="18"/>
-      <c r="C9" s="21"/>
+      <c r="A9" s="23"/>
+      <c r="B9" s="44"/>
+      <c r="C9" s="38"/>
       <c r="D9" s="6">
         <v>2</v>
       </c>
@@ -1395,9 +1405,9 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="15"/>
-      <c r="B10" s="18"/>
-      <c r="C10" s="21"/>
+      <c r="A10" s="23"/>
+      <c r="B10" s="44"/>
+      <c r="C10" s="38"/>
       <c r="D10" s="6">
         <v>3</v>
       </c>
@@ -1406,9 +1416,9 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="15"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="21"/>
+      <c r="A11" s="23"/>
+      <c r="B11" s="44"/>
+      <c r="C11" s="38"/>
       <c r="D11" s="6">
         <v>4</v>
       </c>
@@ -1417,9 +1427,9 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="15"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="21"/>
+      <c r="A12" s="23"/>
+      <c r="B12" s="44"/>
+      <c r="C12" s="38"/>
       <c r="D12" s="6">
         <v>5</v>
       </c>
@@ -1428,9 +1438,9 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="15"/>
-      <c r="B13" s="18"/>
-      <c r="C13" s="21"/>
+      <c r="A13" s="23"/>
+      <c r="B13" s="44"/>
+      <c r="C13" s="38"/>
       <c r="D13" s="6">
         <v>6</v>
       </c>
@@ -1439,9 +1449,9 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="15"/>
-      <c r="B14" s="18"/>
-      <c r="C14" s="21"/>
+      <c r="A14" s="23"/>
+      <c r="B14" s="44"/>
+      <c r="C14" s="38"/>
       <c r="D14" s="6">
         <v>7</v>
       </c>
@@ -1450,9 +1460,9 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="15"/>
-      <c r="B15" s="18"/>
-      <c r="C15" s="21"/>
+      <c r="A15" s="23"/>
+      <c r="B15" s="44"/>
+      <c r="C15" s="38"/>
       <c r="D15" s="6">
         <v>8</v>
       </c>
@@ -1461,9 +1471,9 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="15"/>
-      <c r="B16" s="18"/>
-      <c r="C16" s="21"/>
+      <c r="A16" s="23"/>
+      <c r="B16" s="44"/>
+      <c r="C16" s="38"/>
       <c r="D16" s="6">
         <v>9</v>
       </c>
@@ -1472,9 +1482,9 @@
       </c>
     </row>
     <row r="17" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="15"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="21"/>
+      <c r="A17" s="23"/>
+      <c r="B17" s="44"/>
+      <c r="C17" s="38"/>
       <c r="D17" s="6">
         <v>10</v>
       </c>
@@ -1483,9 +1493,9 @@
       </c>
     </row>
     <row r="18" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="15"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="21"/>
+      <c r="A18" s="23"/>
+      <c r="B18" s="44"/>
+      <c r="C18" s="38"/>
       <c r="D18" s="6">
         <v>11</v>
       </c>
@@ -1494,9 +1504,9 @@
       </c>
     </row>
     <row r="19" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="16"/>
-      <c r="B19" s="19"/>
-      <c r="C19" s="22"/>
+      <c r="A19" s="24"/>
+      <c r="B19" s="31"/>
+      <c r="C19" s="39"/>
       <c r="D19" s="5">
         <v>12</v>
       </c>
@@ -1505,13 +1515,13 @@
       </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A20" s="14" t="s">
+      <c r="A20" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B20" s="14" t="s">
+      <c r="B20" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C20" s="20" t="s">
+      <c r="C20" s="37" t="s">
         <v>33</v>
       </c>
       <c r="D20" s="4">
@@ -1522,9 +1532,9 @@
       </c>
     </row>
     <row r="21" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="15"/>
-      <c r="B21" s="15"/>
-      <c r="C21" s="21"/>
+      <c r="A21" s="23"/>
+      <c r="B21" s="23"/>
+      <c r="C21" s="38"/>
       <c r="D21" s="6">
         <v>2</v>
       </c>
@@ -1533,9 +1543,9 @@
       </c>
     </row>
     <row r="22" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="15"/>
-      <c r="B22" s="15"/>
-      <c r="C22" s="21"/>
+      <c r="A22" s="23"/>
+      <c r="B22" s="23"/>
+      <c r="C22" s="38"/>
       <c r="D22" s="6">
         <v>3</v>
       </c>
@@ -1544,9 +1554,9 @@
       </c>
     </row>
     <row r="23" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="15"/>
-      <c r="B23" s="15"/>
-      <c r="C23" s="21"/>
+      <c r="A23" s="23"/>
+      <c r="B23" s="23"/>
+      <c r="C23" s="38"/>
       <c r="D23" s="6">
         <v>4</v>
       </c>
@@ -1555,9 +1565,9 @@
       </c>
     </row>
     <row r="24" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="15"/>
-      <c r="B24" s="15"/>
-      <c r="C24" s="21"/>
+      <c r="A24" s="23"/>
+      <c r="B24" s="23"/>
+      <c r="C24" s="38"/>
       <c r="D24" s="6">
         <v>5</v>
       </c>
@@ -1566,9 +1576,9 @@
       </c>
     </row>
     <row r="25" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="15"/>
-      <c r="B25" s="15"/>
-      <c r="C25" s="21"/>
+      <c r="A25" s="23"/>
+      <c r="B25" s="23"/>
+      <c r="C25" s="38"/>
       <c r="D25" s="6">
         <v>6</v>
       </c>
@@ -1577,9 +1587,9 @@
       </c>
     </row>
     <row r="26" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="16"/>
-      <c r="B26" s="16"/>
-      <c r="C26" s="22"/>
+      <c r="A26" s="24"/>
+      <c r="B26" s="24"/>
+      <c r="C26" s="39"/>
       <c r="D26" s="5">
         <v>7</v>
       </c>
@@ -1588,13 +1598,13 @@
       </c>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A27" s="14" t="s">
+      <c r="A27" s="22" t="s">
         <v>8</v>
       </c>
-      <c r="B27" s="14" t="s">
+      <c r="B27" s="22" t="s">
         <v>48</v>
       </c>
-      <c r="C27" s="20" t="s">
+      <c r="C27" s="37" t="s">
         <v>41</v>
       </c>
       <c r="D27" s="4">
@@ -1605,9 +1615,9 @@
       </c>
     </row>
     <row r="28" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="15"/>
-      <c r="B28" s="15"/>
-      <c r="C28" s="21"/>
+      <c r="A28" s="23"/>
+      <c r="B28" s="23"/>
+      <c r="C28" s="38"/>
       <c r="D28" s="6">
         <v>2</v>
       </c>
@@ -1616,9 +1626,9 @@
       </c>
     </row>
     <row r="29" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="15"/>
-      <c r="B29" s="15"/>
-      <c r="C29" s="21"/>
+      <c r="A29" s="23"/>
+      <c r="B29" s="23"/>
+      <c r="C29" s="38"/>
       <c r="D29" s="6">
         <v>3</v>
       </c>
@@ -1627,9 +1637,9 @@
       </c>
     </row>
     <row r="30" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="15"/>
-      <c r="B30" s="15"/>
-      <c r="C30" s="21"/>
+      <c r="A30" s="23"/>
+      <c r="B30" s="23"/>
+      <c r="C30" s="38"/>
       <c r="D30" s="6">
         <v>4</v>
       </c>
@@ -1638,9 +1648,9 @@
       </c>
     </row>
     <row r="31" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="15"/>
-      <c r="B31" s="15"/>
-      <c r="C31" s="21"/>
+      <c r="A31" s="23"/>
+      <c r="B31" s="23"/>
+      <c r="C31" s="38"/>
       <c r="D31" s="6">
         <v>5</v>
       </c>
@@ -1649,9 +1659,9 @@
       </c>
     </row>
     <row r="32" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="16"/>
-      <c r="B32" s="16"/>
-      <c r="C32" s="22"/>
+      <c r="A32" s="24"/>
+      <c r="B32" s="24"/>
+      <c r="C32" s="39"/>
       <c r="D32" s="5">
         <v>6</v>
       </c>
@@ -1660,13 +1670,13 @@
       </c>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A33" s="14" t="s">
+      <c r="A33" s="22" t="s">
         <v>12</v>
       </c>
-      <c r="B33" s="25" t="s">
+      <c r="B33" s="27" t="s">
         <v>142</v>
       </c>
-      <c r="C33" s="20" t="s">
+      <c r="C33" s="37" t="s">
         <v>151</v>
       </c>
       <c r="D33" s="4">
@@ -1677,9 +1687,9 @@
       </c>
     </row>
     <row r="34" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="15"/>
-      <c r="B34" s="26"/>
-      <c r="C34" s="21"/>
+      <c r="A34" s="23"/>
+      <c r="B34" s="28"/>
+      <c r="C34" s="38"/>
       <c r="D34" s="6">
         <v>1</v>
       </c>
@@ -1688,9 +1698,9 @@
       </c>
     </row>
     <row r="35" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="15"/>
-      <c r="B35" s="26"/>
-      <c r="C35" s="21"/>
+      <c r="A35" s="23"/>
+      <c r="B35" s="28"/>
+      <c r="C35" s="38"/>
       <c r="D35" s="6">
         <v>2</v>
       </c>
@@ -1699,9 +1709,9 @@
       </c>
     </row>
     <row r="36" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="15"/>
-      <c r="B36" s="26"/>
-      <c r="C36" s="21"/>
+      <c r="A36" s="23"/>
+      <c r="B36" s="28"/>
+      <c r="C36" s="38"/>
       <c r="D36" s="6">
         <v>3</v>
       </c>
@@ -1710,9 +1720,9 @@
       </c>
     </row>
     <row r="37" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="15"/>
-      <c r="B37" s="26"/>
-      <c r="C37" s="21"/>
+      <c r="A37" s="23"/>
+      <c r="B37" s="28"/>
+      <c r="C37" s="38"/>
       <c r="D37" s="6">
         <v>4</v>
       </c>
@@ -1721,9 +1731,9 @@
       </c>
     </row>
     <row r="38" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="15"/>
-      <c r="B38" s="26"/>
-      <c r="C38" s="21"/>
+      <c r="A38" s="23"/>
+      <c r="B38" s="28"/>
+      <c r="C38" s="38"/>
       <c r="D38" s="6">
         <v>5</v>
       </c>
@@ -1732,9 +1742,9 @@
       </c>
     </row>
     <row r="39" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="15"/>
-      <c r="B39" s="26"/>
-      <c r="C39" s="21"/>
+      <c r="A39" s="23"/>
+      <c r="B39" s="28"/>
+      <c r="C39" s="38"/>
       <c r="D39" s="6">
         <v>6</v>
       </c>
@@ -1743,9 +1753,9 @@
       </c>
     </row>
     <row r="40" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="16"/>
-      <c r="B40" s="27"/>
-      <c r="C40" s="22"/>
+      <c r="A40" s="24"/>
+      <c r="B40" s="29"/>
+      <c r="C40" s="39"/>
       <c r="D40" s="5">
         <v>9</v>
       </c>
@@ -1754,13 +1764,13 @@
       </c>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A41" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B41" s="23" t="s">
+      <c r="A41" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B41" s="25" t="s">
         <v>51</v>
       </c>
-      <c r="C41" s="20" t="s">
+      <c r="C41" s="37" t="s">
         <v>49</v>
       </c>
       <c r="D41" s="4">
@@ -1774,9 +1784,9 @@
       </c>
     </row>
     <row r="42" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="16"/>
-      <c r="B42" s="24"/>
-      <c r="C42" s="22"/>
+      <c r="A42" s="24"/>
+      <c r="B42" s="26"/>
+      <c r="C42" s="39"/>
       <c r="D42" s="5">
         <v>2</v>
       </c>
@@ -1785,13 +1795,13 @@
       </c>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A43" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B43" s="23" t="s">
+      <c r="A43" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B43" s="25" t="s">
         <v>53</v>
       </c>
-      <c r="C43" s="20" t="s">
+      <c r="C43" s="37" t="s">
         <v>52</v>
       </c>
       <c r="D43" s="4">
@@ -1805,9 +1815,9 @@
       </c>
     </row>
     <row r="44" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="16"/>
-      <c r="B44" s="24"/>
-      <c r="C44" s="22"/>
+      <c r="A44" s="24"/>
+      <c r="B44" s="26"/>
+      <c r="C44" s="39"/>
       <c r="D44" s="5">
         <v>2</v>
       </c>
@@ -1816,13 +1826,13 @@
       </c>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A45" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B45" s="23" t="s">
+      <c r="A45" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B45" s="25" t="s">
         <v>55</v>
       </c>
-      <c r="C45" s="20" t="s">
+      <c r="C45" s="37" t="s">
         <v>54</v>
       </c>
       <c r="D45" s="4">
@@ -1836,9 +1846,9 @@
       </c>
     </row>
     <row r="46" spans="1:6" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="16"/>
-      <c r="B46" s="24"/>
-      <c r="C46" s="22"/>
+      <c r="A46" s="24"/>
+      <c r="B46" s="26"/>
+      <c r="C46" s="39"/>
       <c r="D46" s="5">
         <v>2</v>
       </c>
@@ -1850,13 +1860,13 @@
       </c>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A47" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B47" s="23" t="s">
+      <c r="A47" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B47" s="25" t="s">
         <v>69</v>
       </c>
-      <c r="C47" s="28" t="s">
+      <c r="C47" s="42" t="s">
         <v>80</v>
       </c>
       <c r="D47" s="4">
@@ -1870,13 +1880,13 @@
       </c>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A48" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B48" s="24" t="s">
+      <c r="A48" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B48" s="26" t="s">
         <v>69</v>
       </c>
-      <c r="C48" s="29"/>
+      <c r="C48" s="43"/>
       <c r="D48" s="5">
         <v>2</v>
       </c>
@@ -1888,13 +1898,13 @@
       </c>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A49" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B49" s="23" t="s">
+      <c r="A49" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B49" s="25" t="s">
         <v>70</v>
       </c>
-      <c r="C49" s="20" t="s">
+      <c r="C49" s="37" t="s">
         <v>81</v>
       </c>
       <c r="D49" s="4">
@@ -1908,13 +1918,13 @@
       </c>
     </row>
     <row r="50" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A50" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B50" s="24" t="s">
+      <c r="A50" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B50" s="26" t="s">
         <v>70</v>
       </c>
-      <c r="C50" s="22"/>
+      <c r="C50" s="39"/>
       <c r="D50" s="5">
         <v>2</v>
       </c>
@@ -1926,13 +1936,13 @@
       </c>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A51" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B51" s="23" t="s">
+      <c r="A51" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B51" s="25" t="s">
         <v>71</v>
       </c>
-      <c r="C51" s="20" t="s">
+      <c r="C51" s="37" t="s">
         <v>82</v>
       </c>
       <c r="D51" s="4">
@@ -1946,13 +1956,13 @@
       </c>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A52" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B52" s="24" t="s">
+      <c r="A52" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B52" s="26" t="s">
         <v>71</v>
       </c>
-      <c r="C52" s="22"/>
+      <c r="C52" s="39"/>
       <c r="D52" s="5">
         <v>2</v>
       </c>
@@ -1964,13 +1974,13 @@
       </c>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A53" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B53" s="23" t="s">
+      <c r="A53" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B53" s="25" t="s">
         <v>72</v>
       </c>
-      <c r="C53" s="28" t="s">
+      <c r="C53" s="42" t="s">
         <v>83</v>
       </c>
       <c r="D53" s="4">
@@ -1984,13 +1994,13 @@
       </c>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A54" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B54" s="24" t="s">
+      <c r="A54" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B54" s="26" t="s">
         <v>72</v>
       </c>
-      <c r="C54" s="29"/>
+      <c r="C54" s="43"/>
       <c r="D54" s="5">
         <v>2</v>
       </c>
@@ -2002,13 +2012,13 @@
       </c>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A55" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B55" s="23" t="s">
+      <c r="A55" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B55" s="25" t="s">
         <v>73</v>
       </c>
-      <c r="C55" s="20" t="s">
+      <c r="C55" s="37" t="s">
         <v>84</v>
       </c>
       <c r="D55" s="4">
@@ -2022,13 +2032,13 @@
       </c>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A56" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B56" s="24" t="s">
+      <c r="A56" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B56" s="26" t="s">
         <v>73</v>
       </c>
-      <c r="C56" s="22"/>
+      <c r="C56" s="39"/>
       <c r="D56" s="5">
         <v>2</v>
       </c>
@@ -2040,13 +2050,13 @@
       </c>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A57" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B57" s="23" t="s">
+      <c r="A57" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B57" s="25" t="s">
         <v>74</v>
       </c>
-      <c r="C57" s="28" t="s">
+      <c r="C57" s="42" t="s">
         <v>85</v>
       </c>
       <c r="D57" s="4">
@@ -2060,13 +2070,13 @@
       </c>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A58" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B58" s="24" t="s">
+      <c r="A58" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B58" s="26" t="s">
         <v>74</v>
       </c>
-      <c r="C58" s="29"/>
+      <c r="C58" s="43"/>
       <c r="D58" s="5">
         <v>2</v>
       </c>
@@ -2078,13 +2088,13 @@
       </c>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A59" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B59" s="23" t="s">
+      <c r="A59" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B59" s="25" t="s">
         <v>75</v>
       </c>
-      <c r="C59" s="28" t="s">
+      <c r="C59" s="42" t="s">
         <v>86</v>
       </c>
       <c r="D59" s="4">
@@ -2098,13 +2108,13 @@
       </c>
     </row>
     <row r="60" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A60" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B60" s="24" t="s">
+      <c r="A60" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B60" s="26" t="s">
         <v>75</v>
       </c>
-      <c r="C60" s="29"/>
+      <c r="C60" s="43"/>
       <c r="D60" s="5">
         <v>2</v>
       </c>
@@ -2116,13 +2126,13 @@
       </c>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A61" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B61" s="23" t="s">
+      <c r="A61" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B61" s="25" t="s">
         <v>76</v>
       </c>
-      <c r="C61" s="20" t="s">
+      <c r="C61" s="37" t="s">
         <v>87</v>
       </c>
       <c r="D61" s="4">
@@ -2136,13 +2146,13 @@
       </c>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A62" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B62" s="24" t="s">
+      <c r="A62" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B62" s="26" t="s">
         <v>76</v>
       </c>
-      <c r="C62" s="22"/>
+      <c r="C62" s="39"/>
       <c r="D62" s="5">
         <v>2</v>
       </c>
@@ -2154,13 +2164,13 @@
       </c>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A63" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B63" s="23" t="s">
+      <c r="A63" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B63" s="25" t="s">
         <v>77</v>
       </c>
-      <c r="C63" s="20" t="s">
+      <c r="C63" s="37" t="s">
         <v>88</v>
       </c>
       <c r="D63" s="4">
@@ -2174,13 +2184,13 @@
       </c>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A64" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B64" s="24" t="s">
+      <c r="A64" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B64" s="26" t="s">
         <v>77</v>
       </c>
-      <c r="C64" s="22"/>
+      <c r="C64" s="39"/>
       <c r="D64" s="5">
         <v>2</v>
       </c>
@@ -2192,13 +2202,13 @@
       </c>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A65" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B65" s="23" t="s">
+      <c r="A65" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B65" s="25" t="s">
         <v>78</v>
       </c>
-      <c r="C65" s="20" t="s">
+      <c r="C65" s="37" t="s">
         <v>89</v>
       </c>
       <c r="D65" s="4">
@@ -2212,13 +2222,13 @@
       </c>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A66" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B66" s="24" t="s">
+      <c r="A66" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B66" s="26" t="s">
         <v>78</v>
       </c>
-      <c r="C66" s="22"/>
+      <c r="C66" s="39"/>
       <c r="D66" s="5">
         <v>2</v>
       </c>
@@ -2230,13 +2240,13 @@
       </c>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A67" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B67" s="23" t="s">
+      <c r="A67" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B67" s="25" t="s">
         <v>79</v>
       </c>
-      <c r="C67" s="20" t="s">
+      <c r="C67" s="37" t="s">
         <v>90</v>
       </c>
       <c r="D67" s="7">
@@ -2250,13 +2260,13 @@
       </c>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A68" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B68" s="24" t="s">
+      <c r="A68" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B68" s="26" t="s">
         <v>79</v>
       </c>
-      <c r="C68" s="22"/>
+      <c r="C68" s="39"/>
       <c r="D68" s="5">
         <v>2</v>
       </c>
@@ -2265,13 +2275,13 @@
       </c>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A69" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B69" s="23" t="s">
+      <c r="A69" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B69" s="25" t="s">
         <v>65</v>
       </c>
-      <c r="C69" s="20" t="s">
+      <c r="C69" s="37" t="s">
         <v>56</v>
       </c>
       <c r="D69" s="4">
@@ -2285,13 +2295,13 @@
       </c>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A70" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B70" s="24" t="s">
+      <c r="A70" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B70" s="26" t="s">
         <v>65</v>
       </c>
-      <c r="C70" s="22"/>
+      <c r="C70" s="39"/>
       <c r="D70" s="5">
         <v>2</v>
       </c>
@@ -2303,13 +2313,13 @@
       </c>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A71" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B71" s="23" t="s">
+      <c r="A71" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B71" s="25" t="s">
         <v>66</v>
       </c>
-      <c r="C71" s="20" t="s">
+      <c r="C71" s="37" t="s">
         <v>91</v>
       </c>
       <c r="D71" s="4">
@@ -2323,13 +2333,13 @@
       </c>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A72" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B72" s="24" t="s">
+      <c r="A72" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B72" s="26" t="s">
         <v>66</v>
       </c>
-      <c r="C72" s="22"/>
+      <c r="C72" s="39"/>
       <c r="D72" s="5">
         <v>2</v>
       </c>
@@ -2341,13 +2351,13 @@
       </c>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A73" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B73" s="23" t="s">
+      <c r="A73" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B73" s="25" t="s">
         <v>67</v>
       </c>
-      <c r="C73" s="20" t="s">
+      <c r="C73" s="37" t="s">
         <v>92</v>
       </c>
       <c r="D73" s="4">
@@ -2361,13 +2371,13 @@
       </c>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A74" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B74" s="24" t="s">
+      <c r="A74" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B74" s="26" t="s">
         <v>67</v>
       </c>
-      <c r="C74" s="22"/>
+      <c r="C74" s="39"/>
       <c r="D74" s="5">
         <v>2</v>
       </c>
@@ -2379,13 +2389,13 @@
       </c>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A75" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B75" s="23" t="s">
+      <c r="A75" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B75" s="25" t="s">
         <v>68</v>
       </c>
-      <c r="C75" s="20" t="s">
+      <c r="C75" s="37" t="s">
         <v>93</v>
       </c>
       <c r="D75" s="4">
@@ -2399,13 +2409,13 @@
       </c>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A76" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B76" s="24" t="s">
+      <c r="A76" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B76" s="26" t="s">
         <v>68</v>
       </c>
-      <c r="C76" s="22"/>
+      <c r="C76" s="39"/>
       <c r="D76" s="5">
         <v>2</v>
       </c>
@@ -2417,13 +2427,13 @@
       </c>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A77" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B77" s="23" t="s">
+      <c r="A77" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B77" s="25" t="s">
         <v>60</v>
       </c>
-      <c r="C77" s="28" t="s">
+      <c r="C77" s="42" t="s">
         <v>94</v>
       </c>
       <c r="D77" s="4">
@@ -2437,13 +2447,13 @@
       </c>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A78" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B78" s="24" t="s">
+      <c r="A78" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B78" s="26" t="s">
         <v>60</v>
       </c>
-      <c r="C78" s="29"/>
+      <c r="C78" s="43"/>
       <c r="D78" s="5">
         <v>2</v>
       </c>
@@ -2455,13 +2465,13 @@
       </c>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A79" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B79" s="23" t="s">
+      <c r="A79" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B79" s="25" t="s">
         <v>61</v>
       </c>
-      <c r="C79" s="20" t="s">
+      <c r="C79" s="37" t="s">
         <v>95</v>
       </c>
       <c r="D79" s="4">
@@ -2475,13 +2485,13 @@
       </c>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A80" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B80" s="24" t="s">
+      <c r="A80" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B80" s="26" t="s">
         <v>61</v>
       </c>
-      <c r="C80" s="22"/>
+      <c r="C80" s="39"/>
       <c r="D80" s="5">
         <v>2</v>
       </c>
@@ -2493,13 +2503,13 @@
       </c>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A81" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B81" s="23" t="s">
+      <c r="A81" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B81" s="25" t="s">
         <v>62</v>
       </c>
-      <c r="C81" s="20" t="s">
+      <c r="C81" s="37" t="s">
         <v>96</v>
       </c>
       <c r="D81" s="4">
@@ -2513,13 +2523,13 @@
       </c>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A82" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B82" s="24" t="s">
+      <c r="A82" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B82" s="26" t="s">
         <v>62</v>
       </c>
-      <c r="C82" s="22"/>
+      <c r="C82" s="39"/>
       <c r="D82" s="5">
         <v>2</v>
       </c>
@@ -2531,13 +2541,13 @@
       </c>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A83" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B83" s="23" t="s">
+      <c r="A83" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B83" s="25" t="s">
         <v>63</v>
       </c>
-      <c r="C83" s="28" t="s">
+      <c r="C83" s="42" t="s">
         <v>97</v>
       </c>
       <c r="D83" s="4">
@@ -2551,13 +2561,13 @@
       </c>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A84" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B84" s="24" t="s">
+      <c r="A84" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B84" s="26" t="s">
         <v>63</v>
       </c>
-      <c r="C84" s="29"/>
+      <c r="C84" s="43"/>
       <c r="D84" s="5">
         <v>2</v>
       </c>
@@ -2569,13 +2579,13 @@
       </c>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A85" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B85" s="23" t="s">
+      <c r="A85" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B85" s="25" t="s">
         <v>64</v>
       </c>
-      <c r="C85" s="20" t="s">
+      <c r="C85" s="37" t="s">
         <v>98</v>
       </c>
       <c r="D85" s="4">
@@ -2589,13 +2599,13 @@
       </c>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A86" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B86" s="24" t="s">
+      <c r="A86" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B86" s="26" t="s">
         <v>64</v>
       </c>
-      <c r="C86" s="22"/>
+      <c r="C86" s="39"/>
       <c r="D86" s="5">
         <v>2</v>
       </c>
@@ -2607,13 +2617,13 @@
       </c>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A87" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B87" s="23" t="s">
+      <c r="A87" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B87" s="25" t="s">
         <v>59</v>
       </c>
-      <c r="C87" s="20" t="s">
+      <c r="C87" s="37" t="s">
         <v>99</v>
       </c>
       <c r="D87" s="7">
@@ -2627,13 +2637,13 @@
       </c>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A88" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B88" s="24" t="s">
+      <c r="A88" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B88" s="26" t="s">
         <v>59</v>
       </c>
-      <c r="C88" s="22"/>
+      <c r="C88" s="39"/>
       <c r="D88" s="5">
         <v>2</v>
       </c>
@@ -2642,13 +2652,13 @@
       </c>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A89" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B89" s="17" t="s">
+      <c r="A89" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B89" s="30" t="s">
         <v>101</v>
       </c>
-      <c r="C89" s="20" t="s">
+      <c r="C89" s="37" t="s">
         <v>100</v>
       </c>
       <c r="D89" s="4">
@@ -2659,13 +2669,13 @@
       </c>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A90" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B90" s="19" t="s">
+      <c r="A90" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B90" s="31" t="s">
         <v>101</v>
       </c>
-      <c r="C90" s="22"/>
+      <c r="C90" s="39"/>
       <c r="D90" s="5">
         <v>2</v>
       </c>
@@ -2674,13 +2684,13 @@
       </c>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A91" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B91" s="17" t="s">
+      <c r="A91" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B91" s="30" t="s">
         <v>102</v>
       </c>
-      <c r="C91" s="20" t="s">
+      <c r="C91" s="37" t="s">
         <v>107</v>
       </c>
       <c r="D91" s="4">
@@ -2691,13 +2701,13 @@
       </c>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A92" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B92" s="19" t="s">
+      <c r="A92" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B92" s="31" t="s">
         <v>102</v>
       </c>
-      <c r="C92" s="22"/>
+      <c r="C92" s="39"/>
       <c r="D92" s="5">
         <v>2</v>
       </c>
@@ -2706,13 +2716,13 @@
       </c>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A93" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B93" s="17" t="s">
+      <c r="A93" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B93" s="30" t="s">
         <v>103</v>
       </c>
-      <c r="C93" s="20" t="s">
+      <c r="C93" s="37" t="s">
         <v>108</v>
       </c>
       <c r="D93" s="4">
@@ -2723,13 +2733,13 @@
       </c>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A94" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B94" s="19" t="s">
+      <c r="A94" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B94" s="31" t="s">
         <v>103</v>
       </c>
-      <c r="C94" s="22"/>
+      <c r="C94" s="39"/>
       <c r="D94" s="5">
         <v>2</v>
       </c>
@@ -2738,13 +2748,13 @@
       </c>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A95" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B95" s="17" t="s">
+      <c r="A95" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B95" s="30" t="s">
         <v>104</v>
       </c>
-      <c r="C95" s="20" t="s">
+      <c r="C95" s="37" t="s">
         <v>109</v>
       </c>
       <c r="D95" s="4">
@@ -2755,13 +2765,13 @@
       </c>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A96" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B96" s="19" t="s">
+      <c r="A96" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B96" s="31" t="s">
         <v>104</v>
       </c>
-      <c r="C96" s="22"/>
+      <c r="C96" s="39"/>
       <c r="D96" s="5">
         <v>2</v>
       </c>
@@ -2770,13 +2780,13 @@
       </c>
     </row>
     <row r="97" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A97" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B97" s="17" t="s">
+      <c r="A97" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B97" s="30" t="s">
         <v>105</v>
       </c>
-      <c r="C97" s="20" t="s">
+      <c r="C97" s="37" t="s">
         <v>110</v>
       </c>
       <c r="D97" s="4">
@@ -2787,13 +2797,13 @@
       </c>
     </row>
     <row r="98" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A98" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B98" s="19" t="s">
+      <c r="A98" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B98" s="31" t="s">
         <v>105</v>
       </c>
-      <c r="C98" s="22"/>
+      <c r="C98" s="39"/>
       <c r="D98" s="5">
         <v>2</v>
       </c>
@@ -2802,13 +2812,13 @@
       </c>
     </row>
     <row r="99" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A99" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B99" s="17" t="s">
+      <c r="A99" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B99" s="30" t="s">
         <v>106</v>
       </c>
-      <c r="C99" s="20" t="s">
+      <c r="C99" s="37" t="s">
         <v>111</v>
       </c>
       <c r="D99" s="7">
@@ -2819,13 +2829,13 @@
       </c>
     </row>
     <row r="100" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A100" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B100" s="19" t="s">
+      <c r="A100" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B100" s="31" t="s">
         <v>106</v>
       </c>
-      <c r="C100" s="22"/>
+      <c r="C100" s="39"/>
       <c r="D100" s="5">
         <v>2</v>
       </c>
@@ -2834,13 +2844,13 @@
       </c>
     </row>
     <row r="101" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A101" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B101" s="23" t="s">
+      <c r="A101" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B101" s="25" t="s">
         <v>112</v>
       </c>
-      <c r="C101" s="30" t="s">
+      <c r="C101" s="35" t="s">
         <v>113</v>
       </c>
       <c r="D101" s="4">
@@ -2851,13 +2861,13 @@
       </c>
     </row>
     <row r="102" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A102" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B102" s="24" t="s">
+      <c r="A102" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B102" s="26" t="s">
         <v>112</v>
       </c>
-      <c r="C102" s="31"/>
+      <c r="C102" s="36"/>
       <c r="D102" s="5">
         <v>2</v>
       </c>
@@ -2866,13 +2876,13 @@
       </c>
     </row>
     <row r="103" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A103" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B103" s="25" t="s">
+      <c r="A103" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B103" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="C103" s="20" t="s">
+      <c r="C103" s="37" t="s">
         <v>114</v>
       </c>
       <c r="D103" s="4">
@@ -2883,13 +2893,13 @@
       </c>
     </row>
     <row r="104" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A104" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B104" s="26" t="s">
+      <c r="A104" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B104" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="C104" s="21"/>
+      <c r="C104" s="38"/>
       <c r="D104" s="6">
         <v>2</v>
       </c>
@@ -2898,13 +2908,13 @@
       </c>
     </row>
     <row r="105" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A105" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B105" s="26" t="s">
+      <c r="A105" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B105" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="C105" s="21"/>
+      <c r="C105" s="38"/>
       <c r="D105" s="6">
         <v>3</v>
       </c>
@@ -2913,13 +2923,13 @@
       </c>
     </row>
     <row r="106" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A106" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B106" s="26" t="s">
+      <c r="A106" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B106" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="C106" s="21"/>
+      <c r="C106" s="38"/>
       <c r="D106" s="6">
         <v>4</v>
       </c>
@@ -2928,13 +2938,13 @@
       </c>
     </row>
     <row r="107" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A107" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B107" s="26" t="s">
+      <c r="A107" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B107" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="C107" s="21"/>
+      <c r="C107" s="38"/>
       <c r="D107" s="6">
         <v>5</v>
       </c>
@@ -2943,13 +2953,13 @@
       </c>
     </row>
     <row r="108" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A108" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B108" s="26" t="s">
+      <c r="A108" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B108" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="C108" s="21"/>
+      <c r="C108" s="38"/>
       <c r="D108" s="6">
         <v>6</v>
       </c>
@@ -2958,13 +2968,13 @@
       </c>
     </row>
     <row r="109" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A109" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B109" s="26" t="s">
+      <c r="A109" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B109" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="C109" s="21"/>
+      <c r="C109" s="38"/>
       <c r="D109" s="6">
         <v>7</v>
       </c>
@@ -2973,13 +2983,13 @@
       </c>
     </row>
     <row r="110" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A110" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B110" s="26" t="s">
+      <c r="A110" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B110" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="C110" s="21"/>
+      <c r="C110" s="38"/>
       <c r="D110" s="6">
         <v>8</v>
       </c>
@@ -2988,13 +2998,13 @@
       </c>
     </row>
     <row r="111" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A111" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B111" s="26" t="s">
+      <c r="A111" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B111" s="28" t="s">
         <v>115</v>
       </c>
-      <c r="C111" s="21"/>
+      <c r="C111" s="38"/>
       <c r="D111" s="6">
         <v>9</v>
       </c>
@@ -3003,13 +3013,13 @@
       </c>
     </row>
     <row r="112" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A112" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B112" s="27" t="s">
+      <c r="A112" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B112" s="29" t="s">
         <v>115</v>
       </c>
-      <c r="C112" s="22"/>
+      <c r="C112" s="39"/>
       <c r="D112" s="5">
         <v>99</v>
       </c>
@@ -3018,13 +3028,13 @@
       </c>
     </row>
     <row r="113" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A113" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B113" s="23" t="s">
+      <c r="A113" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B113" s="25" t="s">
         <v>126</v>
       </c>
-      <c r="C113" s="32" t="s">
+      <c r="C113" s="40" t="s">
         <v>128</v>
       </c>
       <c r="D113" s="4">
@@ -3035,13 +3045,13 @@
       </c>
     </row>
     <row r="114" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A114" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B114" s="24" t="s">
+      <c r="A114" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B114" s="26" t="s">
         <v>126</v>
       </c>
-      <c r="C114" s="33"/>
+      <c r="C114" s="41"/>
       <c r="D114" s="5">
         <v>2</v>
       </c>
@@ -3050,13 +3060,13 @@
       </c>
     </row>
     <row r="115" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A115" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B115" s="25" t="s">
+      <c r="A115" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B115" s="27" t="s">
         <v>129</v>
       </c>
-      <c r="C115" s="20" t="s">
+      <c r="C115" s="37" t="s">
         <v>127</v>
       </c>
       <c r="D115" s="4">
@@ -3067,13 +3077,13 @@
       </c>
     </row>
     <row r="116" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A116" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B116" s="26" t="s">
+      <c r="A116" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B116" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="C116" s="21"/>
+      <c r="C116" s="38"/>
       <c r="D116" s="6">
         <v>2</v>
       </c>
@@ -3082,13 +3092,13 @@
       </c>
     </row>
     <row r="117" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A117" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B117" s="26" t="s">
+      <c r="A117" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B117" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="C117" s="21"/>
+      <c r="C117" s="38"/>
       <c r="D117" s="6">
         <v>3</v>
       </c>
@@ -3097,13 +3107,13 @@
       </c>
     </row>
     <row r="118" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A118" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B118" s="26" t="s">
+      <c r="A118" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B118" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="C118" s="21"/>
+      <c r="C118" s="38"/>
       <c r="D118" s="6">
         <v>4</v>
       </c>
@@ -3112,13 +3122,13 @@
       </c>
     </row>
     <row r="119" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A119" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B119" s="26" t="s">
+      <c r="A119" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B119" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="C119" s="21"/>
+      <c r="C119" s="38"/>
       <c r="D119" s="6">
         <v>5</v>
       </c>
@@ -3127,13 +3137,13 @@
       </c>
     </row>
     <row r="120" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A120" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B120" s="26" t="s">
+      <c r="A120" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B120" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="C120" s="21"/>
+      <c r="C120" s="38"/>
       <c r="D120" s="6">
         <v>6</v>
       </c>
@@ -3142,13 +3152,13 @@
       </c>
     </row>
     <row r="121" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A121" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B121" s="26" t="s">
+      <c r="A121" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B121" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="C121" s="21"/>
+      <c r="C121" s="38"/>
       <c r="D121" s="6">
         <v>7</v>
       </c>
@@ -3157,13 +3167,13 @@
       </c>
     </row>
     <row r="122" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A122" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B122" s="26" t="s">
+      <c r="A122" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B122" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="C122" s="21"/>
+      <c r="C122" s="38"/>
       <c r="D122" s="6">
         <v>8</v>
       </c>
@@ -3172,13 +3182,13 @@
       </c>
     </row>
     <row r="123" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A123" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B123" s="26" t="s">
+      <c r="A123" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B123" s="28" t="s">
         <v>129</v>
       </c>
-      <c r="C123" s="21"/>
+      <c r="C123" s="38"/>
       <c r="D123" s="6">
         <v>9</v>
       </c>
@@ -3187,13 +3197,13 @@
       </c>
     </row>
     <row r="124" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A124" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B124" s="27" t="s">
+      <c r="A124" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B124" s="29" t="s">
         <v>129</v>
       </c>
-      <c r="C124" s="22"/>
+      <c r="C124" s="39"/>
       <c r="D124" s="5">
         <v>99</v>
       </c>
@@ -3202,13 +3212,13 @@
       </c>
     </row>
     <row r="125" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A125" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B125" s="23" t="s">
+      <c r="A125" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B125" s="25" t="s">
         <v>131</v>
       </c>
-      <c r="C125" s="32" t="s">
+      <c r="C125" s="40" t="s">
         <v>130</v>
       </c>
       <c r="D125" s="4">
@@ -3219,13 +3229,13 @@
       </c>
     </row>
     <row r="126" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A126" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B126" s="24" t="s">
+      <c r="A126" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B126" s="26" t="s">
         <v>131</v>
       </c>
-      <c r="C126" s="33"/>
+      <c r="C126" s="41"/>
       <c r="D126" s="5">
         <v>2</v>
       </c>
@@ -3234,13 +3244,13 @@
       </c>
     </row>
     <row r="127" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A127" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B127" s="25" t="s">
+      <c r="A127" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B127" s="27" t="s">
         <v>132</v>
       </c>
-      <c r="C127" s="20" t="s">
+      <c r="C127" s="37" t="s">
         <v>133</v>
       </c>
       <c r="D127" s="4">
@@ -3251,13 +3261,13 @@
       </c>
     </row>
     <row r="128" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A128" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B128" s="26" t="s">
+      <c r="A128" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B128" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="C128" s="21"/>
+      <c r="C128" s="38"/>
       <c r="D128" s="6">
         <v>2</v>
       </c>
@@ -3266,13 +3276,13 @@
       </c>
     </row>
     <row r="129" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A129" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B129" s="26" t="s">
+      <c r="A129" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B129" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="C129" s="21"/>
+      <c r="C129" s="38"/>
       <c r="D129" s="6">
         <v>3</v>
       </c>
@@ -3281,13 +3291,13 @@
       </c>
     </row>
     <row r="130" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A130" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B130" s="26" t="s">
+      <c r="A130" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B130" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="C130" s="21"/>
+      <c r="C130" s="38"/>
       <c r="D130" s="6">
         <v>4</v>
       </c>
@@ -3296,13 +3306,13 @@
       </c>
     </row>
     <row r="131" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A131" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B131" s="26" t="s">
+      <c r="A131" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B131" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="C131" s="21"/>
+      <c r="C131" s="38"/>
       <c r="D131" s="6">
         <v>5</v>
       </c>
@@ -3311,13 +3321,13 @@
       </c>
     </row>
     <row r="132" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A132" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B132" s="26" t="s">
+      <c r="A132" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B132" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="C132" s="21"/>
+      <c r="C132" s="38"/>
       <c r="D132" s="6">
         <v>6</v>
       </c>
@@ -3326,13 +3336,13 @@
       </c>
     </row>
     <row r="133" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A133" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B133" s="26" t="s">
+      <c r="A133" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B133" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="C133" s="21"/>
+      <c r="C133" s="38"/>
       <c r="D133" s="6">
         <v>7</v>
       </c>
@@ -3341,13 +3351,13 @@
       </c>
     </row>
     <row r="134" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A134" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B134" s="26" t="s">
+      <c r="A134" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B134" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="C134" s="21"/>
+      <c r="C134" s="38"/>
       <c r="D134" s="6">
         <v>8</v>
       </c>
@@ -3356,13 +3366,13 @@
       </c>
     </row>
     <row r="135" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A135" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B135" s="26" t="s">
+      <c r="A135" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B135" s="28" t="s">
         <v>132</v>
       </c>
-      <c r="C135" s="21"/>
+      <c r="C135" s="38"/>
       <c r="D135" s="6">
         <v>9</v>
       </c>
@@ -3371,13 +3381,13 @@
       </c>
     </row>
     <row r="136" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A136" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B136" s="27" t="s">
+      <c r="A136" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B136" s="29" t="s">
         <v>132</v>
       </c>
-      <c r="C136" s="22"/>
+      <c r="C136" s="39"/>
       <c r="D136" s="5">
         <v>99</v>
       </c>
@@ -3386,13 +3396,13 @@
       </c>
     </row>
     <row r="137" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A137" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B137" s="23" t="s">
+      <c r="A137" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B137" s="25" t="s">
         <v>136</v>
       </c>
-      <c r="C137" s="30" t="s">
+      <c r="C137" s="35" t="s">
         <v>134</v>
       </c>
       <c r="D137" s="4">
@@ -3403,13 +3413,13 @@
       </c>
     </row>
     <row r="138" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A138" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B138" s="24" t="s">
+      <c r="A138" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B138" s="26" t="s">
         <v>136</v>
       </c>
-      <c r="C138" s="31"/>
+      <c r="C138" s="36"/>
       <c r="D138" s="5">
         <v>2</v>
       </c>
@@ -3418,13 +3428,13 @@
       </c>
     </row>
     <row r="139" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A139" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B139" s="25" t="s">
+      <c r="A139" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B139" s="27" t="s">
         <v>137</v>
       </c>
-      <c r="C139" s="20" t="s">
+      <c r="C139" s="37" t="s">
         <v>135</v>
       </c>
       <c r="D139" s="4">
@@ -3435,13 +3445,13 @@
       </c>
     </row>
     <row r="140" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A140" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B140" s="26" t="s">
+      <c r="A140" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B140" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="C140" s="21"/>
+      <c r="C140" s="38"/>
       <c r="D140" s="6">
         <v>2</v>
       </c>
@@ -3450,13 +3460,13 @@
       </c>
     </row>
     <row r="141" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A141" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B141" s="26" t="s">
+      <c r="A141" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B141" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="C141" s="21"/>
+      <c r="C141" s="38"/>
       <c r="D141" s="6">
         <v>3</v>
       </c>
@@ -3465,13 +3475,13 @@
       </c>
     </row>
     <row r="142" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A142" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B142" s="26" t="s">
+      <c r="A142" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B142" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="C142" s="21"/>
+      <c r="C142" s="38"/>
       <c r="D142" s="6">
         <v>4</v>
       </c>
@@ -3480,13 +3490,13 @@
       </c>
     </row>
     <row r="143" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A143" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B143" s="26" t="s">
+      <c r="A143" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B143" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="C143" s="21"/>
+      <c r="C143" s="38"/>
       <c r="D143" s="6">
         <v>5</v>
       </c>
@@ -3495,13 +3505,13 @@
       </c>
     </row>
     <row r="144" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A144" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B144" s="26" t="s">
+      <c r="A144" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B144" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="C144" s="21"/>
+      <c r="C144" s="38"/>
       <c r="D144" s="6">
         <v>6</v>
       </c>
@@ -3510,13 +3520,13 @@
       </c>
     </row>
     <row r="145" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A145" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B145" s="26" t="s">
+      <c r="A145" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B145" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="C145" s="21"/>
+      <c r="C145" s="38"/>
       <c r="D145" s="6">
         <v>7</v>
       </c>
@@ -3525,13 +3535,13 @@
       </c>
     </row>
     <row r="146" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A146" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B146" s="26" t="s">
+      <c r="A146" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B146" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="C146" s="21"/>
+      <c r="C146" s="38"/>
       <c r="D146" s="6">
         <v>8</v>
       </c>
@@ -3540,13 +3550,13 @@
       </c>
     </row>
     <row r="147" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A147" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B147" s="26" t="s">
+      <c r="A147" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B147" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="C147" s="21"/>
+      <c r="C147" s="38"/>
       <c r="D147" s="6">
         <v>9</v>
       </c>
@@ -3555,13 +3565,13 @@
       </c>
     </row>
     <row r="148" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A148" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B148" s="27" t="s">
+      <c r="A148" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B148" s="29" t="s">
         <v>137</v>
       </c>
-      <c r="C148" s="22"/>
+      <c r="C148" s="39"/>
       <c r="D148" s="5">
         <v>99</v>
       </c>
@@ -3570,13 +3580,13 @@
       </c>
     </row>
     <row r="149" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A149" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B149" s="23" t="s">
+      <c r="A149" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B149" s="25" t="s">
         <v>140</v>
       </c>
-      <c r="C149" s="30" t="s">
+      <c r="C149" s="35" t="s">
         <v>138</v>
       </c>
       <c r="D149" s="4">
@@ -3587,13 +3597,13 @@
       </c>
     </row>
     <row r="150" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A150" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B150" s="24" t="s">
+      <c r="A150" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B150" s="26" t="s">
         <v>140</v>
       </c>
-      <c r="C150" s="31"/>
+      <c r="C150" s="36"/>
       <c r="D150" s="5">
         <v>2</v>
       </c>
@@ -3602,13 +3612,13 @@
       </c>
     </row>
     <row r="151" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A151" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B151" s="25" t="s">
+      <c r="A151" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B151" s="27" t="s">
         <v>141</v>
       </c>
-      <c r="C151" s="20" t="s">
+      <c r="C151" s="37" t="s">
         <v>139</v>
       </c>
       <c r="D151" s="4">
@@ -3619,13 +3629,13 @@
       </c>
     </row>
     <row r="152" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A152" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B152" s="26" t="s">
+      <c r="A152" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B152" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="C152" s="21"/>
+      <c r="C152" s="38"/>
       <c r="D152" s="6">
         <v>2</v>
       </c>
@@ -3634,13 +3644,13 @@
       </c>
     </row>
     <row r="153" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A153" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B153" s="26" t="s">
+      <c r="A153" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B153" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="C153" s="21"/>
+      <c r="C153" s="38"/>
       <c r="D153" s="6">
         <v>3</v>
       </c>
@@ -3649,13 +3659,13 @@
       </c>
     </row>
     <row r="154" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A154" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B154" s="26" t="s">
+      <c r="A154" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B154" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="C154" s="21"/>
+      <c r="C154" s="38"/>
       <c r="D154" s="6">
         <v>4</v>
       </c>
@@ -3664,13 +3674,13 @@
       </c>
     </row>
     <row r="155" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A155" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B155" s="26" t="s">
+      <c r="A155" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B155" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="C155" s="21"/>
+      <c r="C155" s="38"/>
       <c r="D155" s="6">
         <v>5</v>
       </c>
@@ -3679,13 +3689,13 @@
       </c>
     </row>
     <row r="156" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A156" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B156" s="26" t="s">
+      <c r="A156" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B156" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="C156" s="21"/>
+      <c r="C156" s="38"/>
       <c r="D156" s="6">
         <v>6</v>
       </c>
@@ -3694,13 +3704,13 @@
       </c>
     </row>
     <row r="157" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A157" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B157" s="26" t="s">
+      <c r="A157" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B157" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="C157" s="21"/>
+      <c r="C157" s="38"/>
       <c r="D157" s="6">
         <v>7</v>
       </c>
@@ -3709,13 +3719,13 @@
       </c>
     </row>
     <row r="158" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A158" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B158" s="26" t="s">
+      <c r="A158" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B158" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="C158" s="21"/>
+      <c r="C158" s="38"/>
       <c r="D158" s="6">
         <v>8</v>
       </c>
@@ -3724,13 +3734,13 @@
       </c>
     </row>
     <row r="159" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A159" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B159" s="26" t="s">
+      <c r="A159" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B159" s="28" t="s">
         <v>141</v>
       </c>
-      <c r="C159" s="21"/>
+      <c r="C159" s="38"/>
       <c r="D159" s="6">
         <v>9</v>
       </c>
@@ -3739,13 +3749,13 @@
       </c>
     </row>
     <row r="160" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A160" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B160" s="27" t="s">
+      <c r="A160" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B160" s="29" t="s">
         <v>141</v>
       </c>
-      <c r="C160" s="22"/>
+      <c r="C160" s="39"/>
       <c r="D160" s="5">
         <v>99</v>
       </c>
@@ -3776,7 +3786,7 @@
       <c r="B162" s="13" t="s">
         <v>154</v>
       </c>
-      <c r="C162" s="9" t="s">
+      <c r="C162" s="45" t="s">
         <v>162</v>
       </c>
       <c r="D162" s="3"/>
@@ -3838,13 +3848,13 @@
       <c r="E166" s="3"/>
     </row>
     <row r="167" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A167" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B167" s="34" t="s">
+      <c r="A167" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B167" s="32" t="s">
         <v>163</v>
       </c>
-      <c r="C167" s="20" t="s">
+      <c r="C167" s="37" t="s">
         <v>170</v>
       </c>
       <c r="D167" s="4">
@@ -3861,13 +3871,13 @@
       </c>
     </row>
     <row r="168" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A168" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B168" s="35" t="s">
+      <c r="A168" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B168" s="33" t="s">
         <v>163</v>
       </c>
-      <c r="C168" s="21"/>
+      <c r="C168" s="38"/>
       <c r="D168" s="6">
         <v>2</v>
       </c>
@@ -3876,13 +3886,13 @@
       </c>
     </row>
     <row r="169" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A169" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B169" s="35" t="s">
+      <c r="A169" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B169" s="33" t="s">
         <v>163</v>
       </c>
-      <c r="C169" s="21"/>
+      <c r="C169" s="38"/>
       <c r="D169" s="6">
         <v>3</v>
       </c>
@@ -3891,13 +3901,13 @@
       </c>
     </row>
     <row r="170" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A170" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B170" s="35" t="s">
+      <c r="A170" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B170" s="33" t="s">
         <v>163</v>
       </c>
-      <c r="C170" s="21"/>
+      <c r="C170" s="38"/>
       <c r="D170" s="6">
         <v>4</v>
       </c>
@@ -3906,13 +3916,13 @@
       </c>
     </row>
     <row r="171" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A171" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B171" s="35" t="s">
+      <c r="A171" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B171" s="33" t="s">
         <v>163</v>
       </c>
-      <c r="C171" s="21"/>
+      <c r="C171" s="38"/>
       <c r="D171" s="6">
         <v>5</v>
       </c>
@@ -3921,13 +3931,13 @@
       </c>
     </row>
     <row r="172" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A172" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B172" s="36" t="s">
+      <c r="A172" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B172" s="34" t="s">
         <v>163</v>
       </c>
-      <c r="C172" s="22"/>
+      <c r="C172" s="39"/>
       <c r="D172" s="5">
         <v>6</v>
       </c>
@@ -3936,13 +3946,13 @@
       </c>
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.2">
-      <c r="A173" s="14" t="s">
-        <v>50</v>
-      </c>
-      <c r="B173" s="34" t="s">
+      <c r="A173" s="22" t="s">
+        <v>50</v>
+      </c>
+      <c r="B173" s="32" t="s">
         <v>171</v>
       </c>
-      <c r="C173" s="20" t="s">
+      <c r="C173" s="37" t="s">
         <v>172</v>
       </c>
       <c r="D173" s="4">
@@ -3959,13 +3969,13 @@
       </c>
     </row>
     <row r="174" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A174" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B174" s="35" t="s">
+      <c r="A174" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B174" s="33" t="s">
         <v>171</v>
       </c>
-      <c r="C174" s="21"/>
+      <c r="C174" s="38"/>
       <c r="D174" s="6">
         <v>2</v>
       </c>
@@ -3974,13 +3984,13 @@
       </c>
     </row>
     <row r="175" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A175" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B175" s="35" t="s">
+      <c r="A175" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B175" s="33" t="s">
         <v>171</v>
       </c>
-      <c r="C175" s="21"/>
+      <c r="C175" s="38"/>
       <c r="D175" s="6">
         <v>3</v>
       </c>
@@ -3989,13 +3999,13 @@
       </c>
     </row>
     <row r="176" spans="1:7" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A176" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B176" s="35" t="s">
+      <c r="A176" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B176" s="33" t="s">
         <v>171</v>
       </c>
-      <c r="C176" s="21"/>
+      <c r="C176" s="38"/>
       <c r="D176" s="6">
         <v>4</v>
       </c>
@@ -4004,13 +4014,13 @@
       </c>
     </row>
     <row r="177" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A177" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B177" s="35" t="s">
+      <c r="A177" s="23" t="s">
+        <v>50</v>
+      </c>
+      <c r="B177" s="33" t="s">
         <v>171</v>
       </c>
-      <c r="C177" s="21"/>
+      <c r="C177" s="38"/>
       <c r="D177" s="6">
         <v>5</v>
       </c>
@@ -4019,13 +4029,13 @@
       </c>
     </row>
     <row r="178" spans="1:5" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A178" s="16" t="s">
-        <v>50</v>
-      </c>
-      <c r="B178" s="36" t="s">
+      <c r="A178" s="24" t="s">
+        <v>50</v>
+      </c>
+      <c r="B178" s="34" t="s">
         <v>171</v>
       </c>
-      <c r="C178" s="22"/>
+      <c r="C178" s="39"/>
       <c r="D178" s="5">
         <v>6</v>
       </c>
@@ -4035,6 +4045,130 @@
     </row>
   </sheetData>
   <mergeCells count="148">
+    <mergeCell ref="A7:A19"/>
+    <mergeCell ref="B7:B19"/>
+    <mergeCell ref="C7:C19"/>
+    <mergeCell ref="C20:C26"/>
+    <mergeCell ref="B20:B26"/>
+    <mergeCell ref="A20:A26"/>
+    <mergeCell ref="A3:A4"/>
+    <mergeCell ref="B3:B4"/>
+    <mergeCell ref="C3:C4"/>
+    <mergeCell ref="A5:A6"/>
+    <mergeCell ref="B5:B6"/>
+    <mergeCell ref="C5:C6"/>
+    <mergeCell ref="B41:B42"/>
+    <mergeCell ref="A41:A42"/>
+    <mergeCell ref="C41:C42"/>
+    <mergeCell ref="C43:C44"/>
+    <mergeCell ref="B43:B44"/>
+    <mergeCell ref="A43:A44"/>
+    <mergeCell ref="A27:A32"/>
+    <mergeCell ref="B27:B32"/>
+    <mergeCell ref="C27:C32"/>
+    <mergeCell ref="C33:C40"/>
+    <mergeCell ref="B33:B40"/>
+    <mergeCell ref="A33:A40"/>
+    <mergeCell ref="A45:A46"/>
+    <mergeCell ref="B45:B46"/>
+    <mergeCell ref="C45:C46"/>
+    <mergeCell ref="C47:C48"/>
+    <mergeCell ref="C49:C50"/>
+    <mergeCell ref="C51:C52"/>
+    <mergeCell ref="B47:B48"/>
+    <mergeCell ref="B49:B50"/>
+    <mergeCell ref="B51:B52"/>
+    <mergeCell ref="A47:A48"/>
+    <mergeCell ref="A49:A50"/>
+    <mergeCell ref="A51:A52"/>
+    <mergeCell ref="C65:C66"/>
+    <mergeCell ref="C67:C68"/>
+    <mergeCell ref="C69:C70"/>
+    <mergeCell ref="C71:C72"/>
+    <mergeCell ref="C73:C74"/>
+    <mergeCell ref="C75:C76"/>
+    <mergeCell ref="C53:C54"/>
+    <mergeCell ref="C55:C56"/>
+    <mergeCell ref="C57:C58"/>
+    <mergeCell ref="C59:C60"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="C63:C64"/>
+    <mergeCell ref="C89:C90"/>
+    <mergeCell ref="C91:C92"/>
+    <mergeCell ref="C93:C94"/>
+    <mergeCell ref="C95:C96"/>
+    <mergeCell ref="C97:C98"/>
+    <mergeCell ref="C99:C100"/>
+    <mergeCell ref="C77:C78"/>
+    <mergeCell ref="C79:C80"/>
+    <mergeCell ref="C81:C82"/>
+    <mergeCell ref="C83:C84"/>
+    <mergeCell ref="C85:C86"/>
+    <mergeCell ref="C87:C88"/>
+    <mergeCell ref="C137:C138"/>
+    <mergeCell ref="C139:C148"/>
+    <mergeCell ref="C149:C150"/>
+    <mergeCell ref="C151:C160"/>
+    <mergeCell ref="C167:C172"/>
+    <mergeCell ref="C173:C178"/>
+    <mergeCell ref="C101:C102"/>
+    <mergeCell ref="C103:C112"/>
+    <mergeCell ref="C113:C114"/>
+    <mergeCell ref="C115:C124"/>
+    <mergeCell ref="C125:C126"/>
+    <mergeCell ref="C127:C136"/>
+    <mergeCell ref="B71:B72"/>
+    <mergeCell ref="B73:B74"/>
+    <mergeCell ref="B75:B76"/>
+    <mergeCell ref="B53:B54"/>
+    <mergeCell ref="B55:B56"/>
+    <mergeCell ref="B57:B58"/>
+    <mergeCell ref="B59:B60"/>
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="B63:B64"/>
+    <mergeCell ref="B151:B160"/>
+    <mergeCell ref="B167:B172"/>
+    <mergeCell ref="B173:B178"/>
+    <mergeCell ref="B101:B102"/>
+    <mergeCell ref="B103:B112"/>
+    <mergeCell ref="B113:B114"/>
+    <mergeCell ref="B115:B124"/>
+    <mergeCell ref="B125:B126"/>
+    <mergeCell ref="B127:B136"/>
+    <mergeCell ref="A53:A54"/>
+    <mergeCell ref="A55:A56"/>
+    <mergeCell ref="A57:A58"/>
+    <mergeCell ref="A59:A60"/>
+    <mergeCell ref="B137:B138"/>
+    <mergeCell ref="B139:B148"/>
+    <mergeCell ref="B149:B150"/>
+    <mergeCell ref="B89:B90"/>
+    <mergeCell ref="B91:B92"/>
+    <mergeCell ref="B93:B94"/>
+    <mergeCell ref="B95:B96"/>
+    <mergeCell ref="B97:B98"/>
+    <mergeCell ref="B99:B100"/>
+    <mergeCell ref="B77:B78"/>
+    <mergeCell ref="B79:B80"/>
+    <mergeCell ref="B81:B82"/>
+    <mergeCell ref="B83:B84"/>
+    <mergeCell ref="B85:B86"/>
+    <mergeCell ref="B87:B88"/>
+    <mergeCell ref="B65:B66"/>
+    <mergeCell ref="B67:B68"/>
+    <mergeCell ref="B69:B70"/>
+    <mergeCell ref="A73:A74"/>
+    <mergeCell ref="A75:A76"/>
+    <mergeCell ref="A77:A78"/>
+    <mergeCell ref="A79:A80"/>
+    <mergeCell ref="A81:A82"/>
+    <mergeCell ref="A83:A84"/>
+    <mergeCell ref="A61:A62"/>
+    <mergeCell ref="A63:A64"/>
+    <mergeCell ref="A65:A66"/>
+    <mergeCell ref="A67:A68"/>
+    <mergeCell ref="A69:A70"/>
+    <mergeCell ref="A71:A72"/>
     <mergeCell ref="G1:G2"/>
     <mergeCell ref="G3:G4"/>
     <mergeCell ref="G5:G6"/>
@@ -4059,130 +4193,6 @@
     <mergeCell ref="A91:A92"/>
     <mergeCell ref="A93:A94"/>
     <mergeCell ref="A95:A96"/>
-    <mergeCell ref="A77:A78"/>
-    <mergeCell ref="A79:A80"/>
-    <mergeCell ref="A81:A82"/>
-    <mergeCell ref="A83:A84"/>
-    <mergeCell ref="A61:A62"/>
-    <mergeCell ref="A63:A64"/>
-    <mergeCell ref="A65:A66"/>
-    <mergeCell ref="A67:A68"/>
-    <mergeCell ref="A69:A70"/>
-    <mergeCell ref="A71:A72"/>
-    <mergeCell ref="A53:A54"/>
-    <mergeCell ref="A55:A56"/>
-    <mergeCell ref="A57:A58"/>
-    <mergeCell ref="A59:A60"/>
-    <mergeCell ref="B137:B138"/>
-    <mergeCell ref="B139:B148"/>
-    <mergeCell ref="B149:B150"/>
-    <mergeCell ref="B89:B90"/>
-    <mergeCell ref="B91:B92"/>
-    <mergeCell ref="B93:B94"/>
-    <mergeCell ref="B95:B96"/>
-    <mergeCell ref="B97:B98"/>
-    <mergeCell ref="B99:B100"/>
-    <mergeCell ref="B77:B78"/>
-    <mergeCell ref="B79:B80"/>
-    <mergeCell ref="B81:B82"/>
-    <mergeCell ref="B83:B84"/>
-    <mergeCell ref="B85:B86"/>
-    <mergeCell ref="B87:B88"/>
-    <mergeCell ref="B65:B66"/>
-    <mergeCell ref="B67:B68"/>
-    <mergeCell ref="B69:B70"/>
-    <mergeCell ref="A73:A74"/>
-    <mergeCell ref="A75:A76"/>
-    <mergeCell ref="B151:B160"/>
-    <mergeCell ref="B167:B172"/>
-    <mergeCell ref="B173:B178"/>
-    <mergeCell ref="B101:B102"/>
-    <mergeCell ref="B103:B112"/>
-    <mergeCell ref="B113:B114"/>
-    <mergeCell ref="B115:B124"/>
-    <mergeCell ref="B125:B126"/>
-    <mergeCell ref="B127:B136"/>
-    <mergeCell ref="B71:B72"/>
-    <mergeCell ref="B73:B74"/>
-    <mergeCell ref="B75:B76"/>
-    <mergeCell ref="B53:B54"/>
-    <mergeCell ref="B55:B56"/>
-    <mergeCell ref="B57:B58"/>
-    <mergeCell ref="B59:B60"/>
-    <mergeCell ref="B61:B62"/>
-    <mergeCell ref="B63:B64"/>
-    <mergeCell ref="C137:C138"/>
-    <mergeCell ref="C139:C148"/>
-    <mergeCell ref="C149:C150"/>
-    <mergeCell ref="C151:C160"/>
-    <mergeCell ref="C167:C172"/>
-    <mergeCell ref="C173:C178"/>
-    <mergeCell ref="C101:C102"/>
-    <mergeCell ref="C103:C112"/>
-    <mergeCell ref="C113:C114"/>
-    <mergeCell ref="C115:C124"/>
-    <mergeCell ref="C125:C126"/>
-    <mergeCell ref="C127:C136"/>
-    <mergeCell ref="C89:C90"/>
-    <mergeCell ref="C91:C92"/>
-    <mergeCell ref="C93:C94"/>
-    <mergeCell ref="C95:C96"/>
-    <mergeCell ref="C97:C98"/>
-    <mergeCell ref="C99:C100"/>
-    <mergeCell ref="C77:C78"/>
-    <mergeCell ref="C79:C80"/>
-    <mergeCell ref="C81:C82"/>
-    <mergeCell ref="C83:C84"/>
-    <mergeCell ref="C85:C86"/>
-    <mergeCell ref="C87:C88"/>
-    <mergeCell ref="C65:C66"/>
-    <mergeCell ref="C67:C68"/>
-    <mergeCell ref="C69:C70"/>
-    <mergeCell ref="C71:C72"/>
-    <mergeCell ref="C73:C74"/>
-    <mergeCell ref="C75:C76"/>
-    <mergeCell ref="C53:C54"/>
-    <mergeCell ref="C55:C56"/>
-    <mergeCell ref="C57:C58"/>
-    <mergeCell ref="C59:C60"/>
-    <mergeCell ref="C61:C62"/>
-    <mergeCell ref="C63:C64"/>
-    <mergeCell ref="A45:A46"/>
-    <mergeCell ref="B45:B46"/>
-    <mergeCell ref="C45:C46"/>
-    <mergeCell ref="C47:C48"/>
-    <mergeCell ref="C49:C50"/>
-    <mergeCell ref="C51:C52"/>
-    <mergeCell ref="B47:B48"/>
-    <mergeCell ref="B49:B50"/>
-    <mergeCell ref="B51:B52"/>
-    <mergeCell ref="A47:A48"/>
-    <mergeCell ref="A49:A50"/>
-    <mergeCell ref="A51:A52"/>
-    <mergeCell ref="B41:B42"/>
-    <mergeCell ref="A41:A42"/>
-    <mergeCell ref="C41:C42"/>
-    <mergeCell ref="C43:C44"/>
-    <mergeCell ref="B43:B44"/>
-    <mergeCell ref="A43:A44"/>
-    <mergeCell ref="A27:A32"/>
-    <mergeCell ref="B27:B32"/>
-    <mergeCell ref="C27:C32"/>
-    <mergeCell ref="C33:C40"/>
-    <mergeCell ref="B33:B40"/>
-    <mergeCell ref="A33:A40"/>
-    <mergeCell ref="A7:A19"/>
-    <mergeCell ref="B7:B19"/>
-    <mergeCell ref="C7:C19"/>
-    <mergeCell ref="C20:C26"/>
-    <mergeCell ref="B20:B26"/>
-    <mergeCell ref="A20:A26"/>
-    <mergeCell ref="A3:A4"/>
-    <mergeCell ref="B3:B4"/>
-    <mergeCell ref="C3:C4"/>
-    <mergeCell ref="A5:A6"/>
-    <mergeCell ref="B5:B6"/>
-    <mergeCell ref="C5:C6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
@@ -4659,6 +4669,21 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010025669DB055EAE143AE39E3D35975AAFD" ma:contentTypeVersion="4" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="ee6a82cd2c03ffce83133c5fff3fb98f">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="2e5a79ae-47ad-41fc-87e1-37324e454923" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="98944c2b906fe05d97cf2899c4b32cd9" ns3:_="">
     <xsd:import namespace="2e5a79ae-47ad-41fc-87e1-37324e454923"/>
@@ -4804,22 +4829,31 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5971854B-A449-4292-9B5E-15B8444343F9}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="2e5a79ae-47ad-41fc-87e1-37324e454923"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D4BDFD4-ED67-42EB-9069-F864BBD9180E}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{02E74FB1-B0BB-446C-BF2B-41528690E251}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4835,28 +4869,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{3D4BDFD4-ED67-42EB-9069-F864BBD9180E}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5971854B-A449-4292-9B5E-15B8444343F9}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="2e5a79ae-47ad-41fc-87e1-37324e454923"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>